<commit_message>
fix the count issue
</commit_message>
<xml_diff>
--- a/wiki_result.xlsx
+++ b/wiki_result.xlsx
@@ -469,7 +469,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>司馬光（1019年11月17日—1086年10月11日），字君實，号迂叟，通称司馬相公，陕州夏县涑水乡（今山西省夏縣）人，祖籍河内郡温县（今河南省焦作市温县），出生于光州光山（今河南省信阳市光山县），北宋政治家、文学家、史学家。西晋安平献王司马孚的后裔。世称涑水先生，身後稱司馬溫公。历仕仁宗、英宗、神宗、哲宗四朝，主持编纂了中国历史上第一部编年体通史《资治通鉴》。
+          <t>司馬光（1019年11月17日—1086年10月11日），字君實，号迂叟，通称司馬相公，陕州夏县涑水乡（今山西省夏縣）人，出生于光州光山（今河南省信阳市光山县），北宋政治家、文学家、史学家。西晋安平献王司马孚的后裔。世称涑水先生，因身後追封溫國公，又稱司馬溫公。历仕仁宗、英宗、神宗、哲宗四朝，主持编纂了中国历史上第一部编年体通史《资治通鉴》。
 == 生平 ==
 === 简介 ===
 宋仁宗时中进士，英宗时进龙图阁直学士。宋神宗时，王安石施行变法，朝廷内外有许多人反对，司马光就是其中之一，引發新舊黨爭。當時司馬光竭力反对王安石变法，与王安石在皇帝前争论，强调祖宗之法不可变。后被命为枢密副使，坚辞不就，次年退居洛阳，以书局自随，专心编纂《通鉴》。
@@ -546,12 +546,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>司馬光（1019年11月17日—1086年10月11日），字君實，号迂叟，通称司馬相公，陕州夏县涑水乡（今山西省夏縣）人，祖籍河内郡温县（今河南省焦作市温县），出生于光州光山（今河南省信阳市光山县），北宋政治家、文学家、史学家。西晋安平献王司马孚的后裔。世称涑水先生，身後稱司馬溫公。历仕仁宗、英宗、神宗、哲宗四朝，主持编纂了中国历史上第一部编年体通史《资治通鉴》。</t>
+          <t>司馬光（1019年11月17日—1086年10月11日），字君實，号迂叟，通称司馬相公，陕州夏县涑水乡（今山西省夏縣）人，出生于光州光山（今河南省信阳市光山县），北宋政治家、文学家、史学家。西晋安平献王司马孚的后裔。世称涑水先生，因身後追封溫國公，又稱司馬溫公。历仕仁宗、英宗、神宗、哲宗四朝，主持编纂了中国历史上第一部编年体通史《资治通鉴》。</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2024-06-20 19:34:02</t>
+          <t>2024-09-28 02:04:46</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2024-06-20 19:34:03</t>
+          <t>2024-09-28 02:04:47</t>
         </is>
       </c>
     </row>
@@ -669,7 +669,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2024-06-20 19:34:04</t>
+          <t>2024-09-28 02:04:48</t>
         </is>
       </c>
     </row>
@@ -705,7 +705,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2024-06-20 19:34:05</t>
+          <t>2024-09-28 02:04:49</t>
         </is>
       </c>
     </row>
@@ -728,7 +728,7 @@
           <t>范純仁（1027年—1101年），字堯夫，蘇州吳縣（今江蘇省蘇州市）人，北宋政治家范仲淹次子。皇祐元年進士，從胡瑗、孫復學。
 == 生平 ==
 范純仁為人正派，政治見解與司馬光同屬保守派。熙寧二年（1069年）七八月間，純仁上書皇上，公開指責安石“掊剋財利”，他因反對王安石變法遭貶逐。但司馬光復相後，堅持要廢除“青苗法”、“免役法”時，范純仁对此不以為然。范純仁對司馬光說：“新法當廢，罷其太甚者可也，恢复差役法一事，尤當熟講而緩行，不然滋為民病。且宰相職在求人，變法非所先也。愿司馬公虛心以延眾議，不必謀自己出。謀自己出，則諂諛得乘間迎合矣！”他希望司馬光虛心“以延眾論”，有可取之處的主張，盡量採納。可惜司馬光並不以此為意，憤怒地說：“子瞻、堯夫之論，光不敢苟同。募役病民害國，百害而無一利，民皆厭而訟之，何其子瞻、堯夫鍾情而不悟！”只把范純仁的看法當作耳邊風，盡廢新法。蘇東坡、范純仁等人相當惆悵地嘆息：“奈何又一位拗相公”。
-范純仁總結自己∶“吾生平所學，得之忠恕二字， 一生用之不盡”。范純仁告誡子弟，德行成就的關鍵就在以“責人之心責己，恕己之心恕人”。范純仁死後諡“忠宣”。妻王質女。有五子范正民、范正平、范正思、范正路及范正國，另有五名女兒分別嫁給將作監主簿崔保孫、朝請郎莊公岳、奉議郎司馬宏、承議郎蔡轂及通直郎郭忠孝。毛斌公之子毛祥公是他的女婿。
+范純仁總結自己∶“吾生平所學，得之忠恕二字， 一生用之不盡”。范純仁告誡子弟，德行成就的關鍵就在以“責人之心責己，恕己之心恕人”。范純仁死後諡“忠宣”。妻王質女。有五子范正民、范正平、范正思、范正路及范正國，另有五名女兒分別嫁給將作監主簿崔保孫、朝請郎莊公岳、奉議郎司馬宏、承議郎蔡轂及通直郎郭忠孝。
 == 著作 ==
 著有《范忠宣公集》五十卷，《臺諫論事》五卷、《邊防奏議》二十卷。文集于南宋嘉定間由沈圻刊印，遂為定本，歷代遞有刊修。現存《范忠宣公集》二十卷，有元天曆元年刊本、明嘉靖間刊本、萬曆三十六年毛一鷺刊二范集本、清康熙合刊二范集本。四庫全書本《范忠宣集》十八巻，奏議二巻遺文一巻補編一巻。
 == 傳記 ==
@@ -745,7 +745,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2024-06-20 19:34:06</t>
+          <t>2024-09-28 02:04:50</t>
         </is>
       </c>
     </row>
@@ -795,7 +795,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2024-06-20 19:34:07</t>
+          <t>2024-09-28 02:04:51</t>
         </is>
       </c>
     </row>
@@ -815,7 +815,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>蘇轍（zhé）（1039年3月18日—1112年10月25日），字子由，一字同叔，晚年自號潁（yǐng）濱遺老，眉州眉山（今四川眉山市）人。宋孝宗淳熙年間，追諡文定。蘇洵之子、蘇軾之弟，北宋嘉祐二年（1057年）與其兄蘇軾同登進士。蘇家父子三人，均在“唐宋八大家”之列，人稱“三蘇”，苏辙則是“小蘇”。作品有《欒城集》傳世，包括《後集》、《三集》，共84卷。
+          <t>蘇轍（zhé）（1039年3月18日—1112年10月25日），字子由，一字同叔，晚年自號潁濱遺老，眉州眉山（今四川眉山市）人。宋孝宗淳熙年間，追諡文定。蘇洵之子、蘇軾之弟，北宋嘉祐二年（1057年）與其兄蘇軾同登進士。蘇家父子三人，均在“唐宋八大家”之列，人稱“三蘇”，苏辙則是“小蘇”。作品有《欒城集》傳世，包括《後集》、《三集》，共84卷。
 == 生平 ==
 宋寶元二年二月二十日（1039年3月18日）蘇轍出生，是蘇洵與程氏的次子。嘉祐二年（1057年），年方十九歲的蘇轍與兄长蘇軾同登進士，轟動京師，不久母喪，返鄉服孝。嘉佑六年（1061年），兄弟二人又同舉制科，苏辙被杨畋推荐至才识兼茂、明于体用科。他在御試制科策中極言朝政得失，司马光将苏辙置于第三等，胡宿“以為不遜，力請黜之”，但是司馬光力舉推荐，並且宋仁宗以“以直言召人，而以直言棄之，天下將謂我何”為由，仍第以四等，除商州軍事推官。後来，因蘇軾任鳳翔簽判，奏請在京侍父。
 英宗治平二年（1065年)出任大名府留守推官，不久差遣管勾大名府路安抚总管司机宜文字。次年蘇洵病逝，终年58岁，苏辙與蘇軾扶喪還蜀安葬。
@@ -862,12 +862,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>蘇轍（zhé）（1039年3月18日—1112年10月25日），字子由，一字同叔，晚年自號潁（yǐng）濱遺老，眉州眉山（今四川眉山市）人。宋孝宗淳熙年間，追諡文定。蘇洵之子、蘇軾之弟，北宋嘉祐二年（1057年）與其兄蘇軾同登進士。蘇家父子三人，均在“唐宋八大家”之列，人稱“三蘇”，苏辙則是“小蘇”。作品有《欒城集》傳世，包括《後集》、《三集》，共84卷。</t>
+          <t>蘇轍（zhé）（1039年3月18日—1112年10月25日），字子由，一字同叔，晚年自號潁濱遺老，眉州眉山（今四川眉山市）人。宋孝宗淳熙年間，追諡文定。蘇洵之子、蘇軾之弟，北宋嘉祐二年（1057年）與其兄蘇軾同登進士。蘇家父子三人，均在“唐宋八大家”之列，人稱“三蘇”，苏辙則是“小蘇”。作品有《欒城集》傳世，包括《後集》、《三集》，共84卷。</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2024-06-20 19:34:07</t>
+          <t>2024-09-28 02:04:52</t>
         </is>
       </c>
     </row>
@@ -904,7 +904,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2024-06-20 19:34:09</t>
+          <t>2024-09-28 02:04:53</t>
         </is>
       </c>
     </row>
@@ -940,7 +940,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2024-06-20 19:34:09</t>
+          <t>2024-09-28 02:04:54</t>
         </is>
       </c>
     </row>
@@ -973,7 +973,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2024-06-20 19:34:10</t>
+          <t>2024-09-28 02:04:55</t>
         </is>
       </c>
     </row>
@@ -1034,7 +1034,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2024-06-20 19:34:11</t>
+          <t>2024-09-28 02:04:56</t>
         </is>
       </c>
     </row>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2024-06-20 19:34:12</t>
+          <t>2024-09-28 02:04:57</t>
         </is>
       </c>
     </row>
@@ -1088,7 +1088,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2024-06-20 19:34:13</t>
+          <t>2024-09-28 02:04:57</t>
         </is>
       </c>
     </row>

</xml_diff>